<commit_message>
Percent totals changed to weighted percents
</commit_message>
<xml_diff>
--- a/Data/CRCP Sediment Data.xlsx
+++ b/Data/CRCP Sediment Data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="123">
   <si>
     <t>Location</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>%Coarse</t>
+  </si>
+  <si>
+    <t>%Fine</t>
   </si>
 </sst>
 </file>
@@ -546,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -585,6 +591,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,27 +789,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CRCP 2014'!$S$3:$S$11</c:f>
+              <c:f>'CRCP 2014'!$U$3:$U$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>6.8169242351573711</c:v>
+                  <c:v>5.4256193335824863</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.492246913273529</c:v>
+                  <c:v>10.649492907419551</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.85961622880367</c:v>
+                  <c:v>10.870859787855965</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.8003059705607249</c:v>
+                  <c:v>9.1215270385317986</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4418987286719549</c:v>
+                  <c:v>9.306930693068642</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="@">
                   <c:v>0</c:v>
@@ -904,27 +911,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CRCP 2014'!$T$3:$T$11</c:f>
+              <c:f>'CRCP 2014'!$V$3:$V$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>62.420584473647665</c:v>
+                  <c:v>73.344304843421611</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.759663110226256</c:v>
+                  <c:v>69.876467744562504</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.265627255343546</c:v>
+                  <c:v>74.567218859597872</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.167598993804276</c:v>
+                  <c:v>39.404007873977626</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83.420942418180346</c:v>
+                  <c:v>86.97920792079222</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="@">
                   <c:v>0</c:v>
@@ -1023,27 +1030,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CRCP 2014'!$U$3:$U$11</c:f>
+              <c:f>'CRCP 2014'!$W$3:$W$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>30.762491291194962</c:v>
+                  <c:v>21.230075822995897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.748089976500218</c:v>
+                  <c:v>19.474039348017943</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.874756515852784</c:v>
+                  <c:v>14.561921352546165</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.032095035635002</c:v>
+                  <c:v>51.474465087490572</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.1371588531476995</c:v>
+                  <c:v>3.7138613861391381</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="@">
                   <c:v>0</c:v>
@@ -1068,8 +1075,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="273859840"/>
-        <c:axId val="273863760"/>
+        <c:axId val="284250856"/>
+        <c:axId val="284252816"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1226,11 +1233,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="273860624"/>
-        <c:axId val="273860232"/>
+        <c:axId val="284253208"/>
+        <c:axId val="284249288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="273859840"/>
+        <c:axId val="284250856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1273,7 +1280,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="273863760"/>
+        <c:crossAx val="284252816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1281,7 +1288,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="273863760"/>
+        <c:axId val="284252816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1332,12 +1339,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="273859840"/>
+        <c:crossAx val="284250856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="273860232"/>
+        <c:axId val="284249288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,12 +1381,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="273860624"/>
+        <c:crossAx val="284253208"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="273860624"/>
+        <c:axId val="284253208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1396,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="273860232"/>
+        <c:crossAx val="284249288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1662,36 +1669,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CRCP 2014'!$S$12:$S$20</c:f>
+              <c:f>'CRCP 2014'!$U$12:$U$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>8.3984322587784455</c:v>
+                  <c:v>7.8982805972832493</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.6876308679348391</c:v>
+                  <c:v>6.2005874481868464</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.3431309039105397</c:v>
+                  <c:v>7.0533018918815067</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.445992825366258</c:v>
+                  <c:v>11.129083922120646</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.6092613501216739</c:v>
+                  <c:v>6.9502374918253045</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.5038503057480384</c:v>
+                  <c:v>7.5664556331634785</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5345932377688403</c:v>
+                  <c:v>5.2010009967070676</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2600171367468018</c:v>
+                  <c:v>4.7441640535098148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.2158206297309349</c:v>
+                  <c:v>9.2209151250943311</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1784,36 +1791,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CRCP 2014'!$T$12:$T$20</c:f>
+              <c:f>'CRCP 2014'!$V$12:$V$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>59.394668063173029</c:v>
+                  <c:v>65.270268889043379</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.251209058172513</c:v>
+                  <c:v>71.749577360060144</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.066618035676271</c:v>
+                  <c:v>77.543736450779789</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.027658898362922</c:v>
+                  <c:v>33.096034182341299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.020587739175127</c:v>
+                  <c:v>85.913315411067586</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75.394418082073258</c:v>
+                  <c:v>77.385532147696992</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87.04230931579886</c:v>
+                  <c:v>89.967463647497638</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>87.401405078070525</c:v>
+                  <c:v>90.875658957941354</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>79.974914353858139</c:v>
+                  <c:v>79.977661499534321</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1903,36 +1910,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CRCP 2014'!$U$12:$U$20</c:f>
+              <c:f>'CRCP 2014'!$W$12:$W$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>32.206899678048529</c:v>
+                  <c:v>26.831450513673378</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.061160073892648</c:v>
+                  <c:v>22.049835191752997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.590251060413181</c:v>
+                  <c:v>15.402961657338704</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.526348276270809</c:v>
+                  <c:v>55.774881895538044</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3701509107031988</c:v>
+                  <c:v>7.1364470971071192</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.101731612178696</c:v>
+                  <c:v>15.048012219139522</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.4230974464323065</c:v>
+                  <c:v>4.8315353557952889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.3385777851826672</c:v>
+                  <c:v>4.3801769885488273</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.809265016410926</c:v>
+                  <c:v>10.801423375371362</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1948,8 +1955,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="273861016"/>
-        <c:axId val="273864152"/>
+        <c:axId val="284254384"/>
+        <c:axId val="284255560"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2032,11 +2039,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="275344912"/>
-        <c:axId val="273864936"/>
+        <c:axId val="285608016"/>
+        <c:axId val="284248504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="273861016"/>
+        <c:axId val="284254384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2079,7 +2086,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="273864152"/>
+        <c:crossAx val="284255560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2087,7 +2094,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="273864152"/>
+        <c:axId val="284255560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2138,12 +2145,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="273861016"/>
+        <c:crossAx val="284254384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="273864936"/>
+        <c:axId val="284248504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2180,12 +2187,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275344912"/>
+        <c:crossAx val="285608016"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="275344912"/>
+        <c:axId val="285608016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2194,7 +2201,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="273864936"/>
+        <c:crossAx val="284248504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3381,14 +3388,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -3411,13 +3418,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>61913</xdr:rowOff>
@@ -3707,13 +3714,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="AG21" sqref="AG21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3722,24 +3730,24 @@
     <col min="2" max="2" width="9.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
       <c r="B1" s="25"/>
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
     </row>
-    <row r="2" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>119</v>
       </c>
@@ -3768,43 +3776,49 @@
         <v>45</v>
       </c>
       <c r="J2" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="M2" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="N2" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="O2" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="P2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="Q2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="R2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="S2" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="T2" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="U2" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="V2" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="U2" s="19" t="s">
+      <c r="W2" s="19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>41703</v>
       </c>
@@ -3835,57 +3849,65 @@
         <f>G3+H3</f>
         <v>7.7379999999999987</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="28">
+        <f>(G3/I3)*100</f>
+        <v>93.266994055311443</v>
+      </c>
+      <c r="K3" s="28">
+        <f>(H3/I3)*100</f>
+        <v>6.73300594468855</v>
+      </c>
+      <c r="L3" s="9">
         <f>April2014LOI!R2</f>
         <v>5.2091110140721781</v>
       </c>
-      <c r="K3" s="9">
+      <c r="M3" s="9">
         <f>April2014LOI!S2</f>
         <v>75.044202786268755</v>
       </c>
-      <c r="L3" s="9">
+      <c r="N3" s="9">
         <f>April2014LOI!T2</f>
         <v>19.746686199659067</v>
       </c>
-      <c r="M3" s="9">
+      <c r="O3" s="9">
         <f>April2014LOI!U2</f>
         <v>8.4247374562425641</v>
       </c>
-      <c r="N3" s="9">
+      <c r="P3" s="9">
         <f>April2014LOI!V2</f>
         <v>49.796966161026575</v>
       </c>
-      <c r="O3" s="9">
+      <c r="Q3" s="9">
         <f>April2014LOI!W2</f>
         <v>41.778296382730858</v>
       </c>
-      <c r="P3" s="10">
-        <f>G3*(L3/100)</f>
+      <c r="R3" s="10">
+        <f>G3*(N3/100)</f>
         <v>1.4251183430293946</v>
       </c>
-      <c r="Q3" s="10">
-        <f>H3*(O3/100)</f>
+      <c r="S3" s="10">
+        <f>H3*(Q3/100)</f>
         <v>0.21766492415402772</v>
       </c>
-      <c r="R3" s="10">
-        <f>P3+Q3</f>
+      <c r="T3" s="10">
+        <f>R3+S3</f>
         <v>1.6427832671834222</v>
       </c>
-      <c r="S3" s="9">
-        <f>(J3+M3)/2</f>
-        <v>6.8169242351573711</v>
-      </c>
-      <c r="T3" s="9">
-        <f>(K3+N3)/2</f>
-        <v>62.420584473647665</v>
-      </c>
       <c r="U3" s="9">
-        <f>(L3+O3)/2</f>
-        <v>30.762491291194962</v>
-      </c>
-      <c r="V3" s="9"/>
+        <f>(L3*$J3/100+O3*$K3/100)</f>
+        <v>5.4256193335824863</v>
+      </c>
+      <c r="V3" s="9">
+        <f>(M3*$J3/100+P3*$K3/100)</f>
+        <v>73.344304843421611</v>
+      </c>
+      <c r="W3" s="9">
+        <f>(N3*$J3/100+Q3*$K3/100)</f>
+        <v>21.230075822995897</v>
+      </c>
+      <c r="X3" s="9"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>41703</v>
       </c>
@@ -3916,56 +3938,65 @@
         <f t="shared" ref="I4:I11" si="0">G4+H4</f>
         <v>2.3820000000000041</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="28">
+        <f t="shared" ref="J4:J8" si="1">(G4/I4)*100</f>
+        <v>94.122586062132683</v>
+      </c>
+      <c r="K4" s="28">
+        <f t="shared" ref="K4:K8" si="2">(H4/I4)*100</f>
+        <v>5.877413937867324</v>
+      </c>
+      <c r="L4" s="9">
         <f>April2014LOI!R4</f>
         <v>10.404026151168784</v>
       </c>
-      <c r="K4" s="9">
+      <c r="M4" s="9">
         <f>April2014LOI!S4</f>
         <v>70.691265697756677</v>
       </c>
-      <c r="L4" s="9">
+      <c r="N4" s="9">
         <f>April2014LOI!T4</f>
         <v>18.904708151074537</v>
       </c>
-      <c r="M4" s="9">
+      <c r="O4" s="9">
         <f>April2014LOI!U4</f>
         <v>14.580467675378273</v>
       </c>
-      <c r="N4" s="9">
+      <c r="P4" s="9">
         <f>April2014LOI!V4</f>
         <v>56.828060522695829</v>
       </c>
-      <c r="O4" s="9">
+      <c r="Q4" s="9">
         <f>April2014LOI!W4</f>
         <v>28.591471801925898</v>
       </c>
-      <c r="P4" s="10">
-        <f t="shared" ref="P4:P11" si="1">G4*(L4/100)</f>
+      <c r="R4" s="10">
+        <f t="shared" ref="R4:R11" si="3">G4*(N4/100)</f>
         <v>0.42384355674709195</v>
       </c>
-      <c r="Q4" s="10">
-        <f t="shared" ref="Q4:Q11" si="2">H4*(O4/100)</f>
+      <c r="S4" s="10">
+        <f t="shared" ref="S4:S11" si="4">H4*(Q4/100)</f>
         <v>4.0028060522696231E-2</v>
       </c>
-      <c r="R4" s="10">
-        <f t="shared" ref="R4:R11" si="3">P4+Q4</f>
+      <c r="T4" s="10">
+        <f t="shared" ref="T4:T11" si="5">R4+S4</f>
         <v>0.46387161726978821</v>
       </c>
-      <c r="S4" s="9">
-        <f t="shared" ref="S4:S11" si="4">(J4+M4)/2</f>
-        <v>12.492246913273529</v>
-      </c>
-      <c r="T4" s="9">
-        <f t="shared" ref="T4:T11" si="5">(K4+N4)/2</f>
-        <v>63.759663110226256</v>
-      </c>
       <c r="U4" s="9">
-        <f t="shared" ref="U4:U11" si="6">(L4+O4)/2</f>
-        <v>23.748089976500218</v>
-      </c>
+        <f t="shared" ref="U4:U6" si="6">(L4*$J4/100+O4*$K4/100)</f>
+        <v>10.649492907419551</v>
+      </c>
+      <c r="V4" s="9">
+        <f t="shared" ref="V4:V6" si="7">(M4*$J4/100+P4*$K4/100)</f>
+        <v>69.876467744562504</v>
+      </c>
+      <c r="W4" s="9">
+        <f t="shared" ref="W4:W6" si="8">(N4*$J4/100+Q4*$K4/100)</f>
+        <v>19.474039348017943</v>
+      </c>
+      <c r="X4" s="9"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>41703</v>
       </c>
@@ -3996,56 +4027,65 @@
         <f t="shared" si="0"/>
         <v>1.9039999999999975</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="28">
+        <f t="shared" si="1"/>
+        <v>88.445378151260485</v>
+      </c>
+      <c r="K5" s="28">
+        <f t="shared" si="2"/>
+        <v>11.55462184873951</v>
+      </c>
+      <c r="L5" s="9">
         <f>April2014LOI!R6</f>
         <v>10.573692551505561</v>
       </c>
-      <c r="K5" s="9">
+      <c r="M5" s="9">
         <f>April2014LOI!S6</f>
         <v>75.258954041204362</v>
       </c>
-      <c r="L5" s="9">
+      <c r="N5" s="9">
         <f>April2014LOI!T6</f>
         <v>14.167353407290078</v>
       </c>
-      <c r="M5" s="9">
+      <c r="O5" s="9">
         <f>April2014LOI!U6</f>
         <v>13.14553990610178</v>
       </c>
-      <c r="N5" s="9">
+      <c r="P5" s="9">
         <f>April2014LOI!V6</f>
         <v>69.27230046948273</v>
       </c>
-      <c r="O5" s="9">
+      <c r="Q5" s="9">
         <f>April2014LOI!W6</f>
         <v>17.582159624415489</v>
       </c>
-      <c r="P5" s="10">
-        <f t="shared" si="1"/>
-        <v>0.23857823137876458</v>
-      </c>
-      <c r="Q5" s="10">
-        <f t="shared" si="2"/>
-        <v>3.868075117371407E-2</v>
-      </c>
       <c r="R5" s="10">
         <f t="shared" si="3"/>
+        <v>0.23857823137876458</v>
+      </c>
+      <c r="S5" s="10">
+        <f t="shared" si="4"/>
+        <v>3.868075117371407E-2</v>
+      </c>
+      <c r="T5" s="10">
+        <f t="shared" si="5"/>
         <v>0.27725898255247866</v>
-      </c>
-      <c r="S5" s="9">
-        <f t="shared" si="4"/>
-        <v>11.85961622880367</v>
-      </c>
-      <c r="T5" s="9">
-        <f t="shared" si="5"/>
-        <v>72.265627255343546</v>
       </c>
       <c r="U5" s="9">
         <f t="shared" si="6"/>
-        <v>15.874756515852784</v>
-      </c>
+        <v>10.870859787855965</v>
+      </c>
+      <c r="V5" s="9">
+        <f t="shared" si="7"/>
+        <v>74.567218859597872</v>
+      </c>
+      <c r="W5" s="9">
+        <f t="shared" si="8"/>
+        <v>14.561921352546165</v>
+      </c>
+      <c r="X5" s="9"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>41703</v>
       </c>
@@ -4076,56 +4116,65 @@
         <f t="shared" si="0"/>
         <v>4.6179999999999914</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="28">
+        <f t="shared" si="1"/>
+        <v>76.266782156777779</v>
+      </c>
+      <c r="K6" s="28">
+        <f t="shared" si="2"/>
+        <v>23.733217843222214</v>
+      </c>
+      <c r="L6" s="9">
         <f>April2014LOI!R8</f>
         <v>9.4117647058824172</v>
       </c>
-      <c r="K6" s="9">
+      <c r="M6" s="9">
         <f>April2014LOI!S8</f>
         <v>44.13533856867673</v>
       </c>
-      <c r="L6" s="9">
+      <c r="N6" s="9">
         <f>April2014LOI!T8</f>
         <v>46.452896725440851</v>
       </c>
-      <c r="M6" s="9">
+      <c r="O6" s="9">
         <f>April2014LOI!U8</f>
         <v>8.1888472352390309</v>
       </c>
-      <c r="N6" s="9">
+      <c r="P6" s="9">
         <f>April2014LOI!V8</f>
         <v>24.199859418931819</v>
       </c>
-      <c r="O6" s="9">
+      <c r="Q6" s="9">
         <f>April2014LOI!W8</f>
         <v>67.611293345829154</v>
       </c>
-      <c r="P6" s="10">
-        <f t="shared" si="1"/>
-        <v>1.6360710226700228</v>
-      </c>
-      <c r="Q6" s="10">
-        <f t="shared" si="2"/>
-        <v>0.74101977507028738</v>
-      </c>
       <c r="R6" s="10">
         <f t="shared" si="3"/>
+        <v>1.6360710226700228</v>
+      </c>
+      <c r="S6" s="10">
+        <f t="shared" si="4"/>
+        <v>0.74101977507028738</v>
+      </c>
+      <c r="T6" s="10">
+        <f t="shared" si="5"/>
         <v>2.3770907977403102</v>
-      </c>
-      <c r="S6" s="9">
-        <f t="shared" si="4"/>
-        <v>8.8003059705607249</v>
-      </c>
-      <c r="T6" s="9">
-        <f t="shared" si="5"/>
-        <v>34.167598993804276</v>
       </c>
       <c r="U6" s="9">
         <f t="shared" si="6"/>
-        <v>57.032095035635002</v>
-      </c>
+        <v>9.1215270385317986</v>
+      </c>
+      <c r="V6" s="9">
+        <f t="shared" si="7"/>
+        <v>39.404007873977626</v>
+      </c>
+      <c r="W6" s="9">
+        <f t="shared" si="8"/>
+        <v>51.474465087490572</v>
+      </c>
+      <c r="X6" s="9"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>41703</v>
       </c>
@@ -4156,56 +4205,63 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="28">
+        <v>0</v>
+      </c>
+      <c r="K7" s="28">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
         <f>April2014LOI!R10</f>
         <v>0</v>
       </c>
-      <c r="K7" s="9">
+      <c r="M7" s="9">
         <f>April2014LOI!S10</f>
         <v>0</v>
       </c>
-      <c r="L7" s="9">
+      <c r="N7" s="9">
         <f>April2014LOI!T10</f>
         <v>0</v>
       </c>
-      <c r="M7" s="9">
+      <c r="O7" s="9">
         <f>April2014LOI!U10</f>
         <v>0</v>
       </c>
-      <c r="N7" s="9">
+      <c r="P7" s="9">
         <f>April2014LOI!V10</f>
         <v>0</v>
       </c>
-      <c r="O7" s="9">
+      <c r="Q7" s="9">
         <f>April2014LOI!W10</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R7" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S7" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="10">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U7" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="U4:U8" si="9">(L7*J7/100+O7*K7/100)</f>
         <v>0</v>
       </c>
+      <c r="V7" s="9">
+        <f t="shared" ref="V4:V11" si="10">(M7+P7)/2</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="9">
+        <f t="shared" ref="W4:W11" si="11">(N7+Q7)/2</f>
+        <v>0</v>
+      </c>
+      <c r="X7" s="9"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>41703</v>
       </c>
@@ -4235,56 +4291,65 @@
         <f t="shared" si="0"/>
         <v>0.16799999999999993</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="28">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="L8" s="9">
         <f>April2014LOI!R12</f>
         <v>7.576866764275267</v>
       </c>
-      <c r="K8" s="9">
+      <c r="M8" s="9">
         <f>April2014LOI!S12</f>
         <v>79.862676915568471</v>
       </c>
-      <c r="L8" s="9">
+      <c r="N8" s="9">
         <f>April2014LOI!T12</f>
         <v>12.560456320156263</v>
       </c>
-      <c r="M8" s="9">
+      <c r="O8" s="9">
         <f>April2014LOI!U12</f>
         <v>9.306930693068642</v>
       </c>
-      <c r="N8" s="9">
+      <c r="P8" s="9">
         <f>April2014LOI!V12</f>
         <v>86.97920792079222</v>
       </c>
-      <c r="O8" s="9">
+      <c r="Q8" s="9">
         <f>April2014LOI!W12</f>
         <v>3.7138613861391381</v>
       </c>
-      <c r="P8" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="10">
-        <f t="shared" si="2"/>
-        <v>6.2392871287137493E-3</v>
-      </c>
       <c r="R8" s="10">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="10">
+        <f t="shared" si="4"/>
         <v>6.2392871287137493E-3</v>
       </c>
-      <c r="S8" s="9">
-        <f t="shared" si="4"/>
-        <v>8.4418987286719549</v>
-      </c>
-      <c r="T8" s="9">
+      <c r="T8" s="10">
         <f t="shared" si="5"/>
-        <v>83.420942418180346</v>
+        <v>6.2392871287137493E-3</v>
       </c>
       <c r="U8" s="9">
-        <f t="shared" si="6"/>
-        <v>8.1371588531476995</v>
-      </c>
+        <f>(L8*$J8/100+O8*$K8/100)</f>
+        <v>9.306930693068642</v>
+      </c>
+      <c r="V8" s="9">
+        <f>(M8*$J8/100+P8*$K8/100)</f>
+        <v>86.97920792079222</v>
+      </c>
+      <c r="W8" s="9">
+        <f>(N8*$J8/100+Q8*$K8/100)</f>
+        <v>3.7138613861391381</v>
+      </c>
+      <c r="X8" s="9"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>41703</v>
       </c>
@@ -4314,20 +4379,20 @@
       <c r="I9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="10" t="str">
+      <c r="J9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="10" t="str">
         <f>April2014!G12</f>
         <v>NAN</v>
       </c>
-      <c r="K9" s="10" t="str">
+      <c r="M9" s="10" t="str">
         <f>April2014!H12</f>
         <v>NAN</v>
       </c>
-      <c r="L9" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="20" t="s">
-        <v>41</v>
-      </c>
       <c r="N9" s="20" t="s">
         <v>41</v>
       </c>
@@ -4352,8 +4417,15 @@
       <c r="U9" s="20" t="s">
         <v>41</v>
       </c>
+      <c r="V9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="W9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="X9" s="9"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>41703</v>
       </c>
@@ -4384,56 +4456,63 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="28">
+        <v>0</v>
+      </c>
+      <c r="K10" s="28">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9">
         <f>April2014LOI!R16</f>
         <v>0</v>
       </c>
-      <c r="K10" s="9">
+      <c r="M10" s="9">
         <f>April2014LOI!S16</f>
         <v>0</v>
       </c>
-      <c r="L10" s="9">
+      <c r="N10" s="9">
         <f>April2014LOI!T16</f>
         <v>0</v>
       </c>
-      <c r="M10" s="9">
+      <c r="O10" s="9">
         <f>April2014LOI!U16</f>
         <v>0</v>
       </c>
-      <c r="N10" s="9">
+      <c r="P10" s="9">
         <f>April2014LOI!V16</f>
         <v>0</v>
       </c>
-      <c r="O10" s="9">
+      <c r="Q10" s="9">
         <f>April2014LOI!W16</f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R10" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S10" s="9">
+      <c r="S10" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="10">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U10" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="U4:U11" si="12">(L10+O10)/2</f>
         <v>0</v>
       </c>
+      <c r="V10" s="9">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X10" s="9"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>41703</v>
       </c>
@@ -4464,56 +4543,63 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="28">
+        <v>0</v>
+      </c>
+      <c r="K11" s="28">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
         <f>April2014LOI!R18</f>
         <v>0</v>
       </c>
-      <c r="K11" s="9">
+      <c r="M11" s="9">
         <f>April2014LOI!S18</f>
         <v>0</v>
       </c>
-      <c r="L11" s="9">
+      <c r="N11" s="9">
         <f>April2014LOI!T18</f>
         <v>0</v>
       </c>
-      <c r="M11" s="9">
+      <c r="O11" s="9">
         <f>April2014LOI!U18</f>
         <v>0</v>
       </c>
-      <c r="N11" s="9">
+      <c r="P11" s="9">
         <f>April2014LOI!V18</f>
         <v>0</v>
       </c>
-      <c r="O11" s="9">
+      <c r="Q11" s="9">
         <f>April2014LOI!W18</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R11" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S11" s="9">
+      <c r="S11" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="10">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U11" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="V11" s="9">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X11" s="9"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>41703</v>
       </c>
@@ -4544,56 +4630,65 @@
         <f>G12+H12</f>
         <v>10.683999999999997</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="28">
+        <f t="shared" ref="J10:J20" si="13">(G12/I12)*100</f>
+        <v>84.902658180456754</v>
+      </c>
+      <c r="K12" s="28">
+        <f t="shared" ref="K10:K20" si="14">(H12/I12)*100</f>
+        <v>15.097341819543248</v>
+      </c>
+      <c r="L12" s="9">
         <f>April2014LOI!R21</f>
         <v>7.6819371727748678</v>
       </c>
-      <c r="K12" s="9">
+      <c r="M12" s="9">
         <f>April2014LOI!S21</f>
         <v>67.81179319371725</v>
       </c>
-      <c r="L12" s="9">
+      <c r="N12" s="9">
         <f>April2014LOI!T21</f>
         <v>24.506269633507884</v>
       </c>
-      <c r="M12" s="9">
+      <c r="O12" s="9">
         <f>April2014LOI!U21</f>
         <v>9.1149273447820232</v>
       </c>
-      <c r="N12" s="9">
+      <c r="P12" s="9">
         <f>April2014LOI!V21</f>
         <v>50.977542932628801</v>
       </c>
-      <c r="O12" s="9">
+      <c r="Q12" s="9">
         <f>April2014LOI!W21</f>
         <v>39.907529722589175</v>
       </c>
-      <c r="P12" s="10">
-        <f>G12*(L12/100)</f>
+      <c r="R12" s="10">
+        <f>G12*(N12/100)</f>
         <v>2.2229637184554996</v>
       </c>
-      <c r="Q12" s="10">
-        <f>H12*(O12/100)</f>
+      <c r="S12" s="10">
+        <f>H12*(Q12/100)</f>
         <v>0.64370845442536351</v>
       </c>
-      <c r="R12" s="10">
-        <f>P12+Q12</f>
+      <c r="T12" s="10">
+        <f>R12+S12</f>
         <v>2.8666721728808628</v>
       </c>
-      <c r="S12" s="9">
-        <f>(J12+M12)/2</f>
-        <v>8.3984322587784455</v>
-      </c>
-      <c r="T12" s="9">
-        <f>(K12+N12)/2</f>
-        <v>59.394668063173029</v>
-      </c>
       <c r="U12" s="9">
-        <f>(L12+O12)/2</f>
-        <v>32.206899678048529</v>
-      </c>
+        <f t="shared" ref="U12:U20" si="15">(L12*$J12/100+O12*$K12/100)</f>
+        <v>7.8982805972832493</v>
+      </c>
+      <c r="V12" s="9">
+        <f t="shared" ref="V12:V20" si="16">(M12*$J12/100+P12*$K12/100)</f>
+        <v>65.270268889043379</v>
+      </c>
+      <c r="W12" s="9">
+        <f t="shared" ref="W12:W20" si="17">(N12*$J12/100+Q12*$K12/100)</f>
+        <v>26.831450513673378</v>
+      </c>
+      <c r="X12" s="9"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>41703</v>
       </c>
@@ -4621,59 +4716,68 @@
         <v>2.6300000000000003</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" ref="I13:I20" si="7">G13+H13</f>
+        <f t="shared" ref="I13:I20" si="18">G13+H13</f>
         <v>46.711999999999996</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="28">
+        <f t="shared" si="13"/>
+        <v>94.369755095050508</v>
+      </c>
+      <c r="K13" s="28">
+        <f t="shared" si="14"/>
+        <v>5.6302449049494792</v>
+      </c>
+      <c r="L13" s="9">
         <f>April2014LOI!R23</f>
         <v>6.011890922376887</v>
       </c>
-      <c r="K13" s="9">
+      <c r="M13" s="9">
         <f>April2014LOI!S23</f>
         <v>72.954860995781686</v>
       </c>
-      <c r="L13" s="9">
+      <c r="N13" s="9">
         <f>April2014LOI!T23</f>
         <v>21.033248081841428</v>
       </c>
-      <c r="M13" s="9">
+      <c r="O13" s="9">
         <f>April2014LOI!U23</f>
         <v>9.3633708134927911</v>
       </c>
-      <c r="N13" s="9">
+      <c r="P13" s="9">
         <f>April2014LOI!V23</f>
         <v>51.54755712056334</v>
       </c>
-      <c r="O13" s="9">
+      <c r="Q13" s="9">
         <f>April2014LOI!W23</f>
         <v>39.089072065943867</v>
       </c>
-      <c r="P13" s="10">
-        <f t="shared" ref="P13:P20" si="8">G13*(L13/100)</f>
+      <c r="R13" s="10">
+        <f t="shared" ref="R13:R20" si="19">G13*(N13/100)</f>
         <v>9.2718764194373371</v>
       </c>
-      <c r="Q13" s="10">
-        <f t="shared" ref="Q13:Q20" si="9">H13*(O13/100)</f>
+      <c r="S13" s="10">
+        <f t="shared" ref="S13:S20" si="20">H13*(Q13/100)</f>
         <v>1.028042595334324</v>
       </c>
-      <c r="R13" s="10">
-        <f t="shared" ref="R13:R20" si="10">P13+Q13</f>
+      <c r="T13" s="10">
+        <f t="shared" ref="T13:T20" si="21">R13+S13</f>
         <v>10.29991901477166</v>
       </c>
-      <c r="S13" s="9">
-        <f t="shared" ref="S13:S20" si="11">(J13+M13)/2</f>
-        <v>7.6876308679348391</v>
-      </c>
-      <c r="T13" s="9">
-        <f t="shared" ref="T13:T20" si="12">(K13+N13)/2</f>
-        <v>62.251209058172513</v>
-      </c>
       <c r="U13" s="9">
-        <f t="shared" ref="U13:U20" si="13">(L13+O13)/2</f>
-        <v>30.061160073892648</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>6.2005874481868464</v>
+      </c>
+      <c r="V13" s="9">
+        <f t="shared" si="16"/>
+        <v>71.749577360060144</v>
+      </c>
+      <c r="W13" s="9">
+        <f t="shared" si="17"/>
+        <v>22.049835191752997</v>
+      </c>
+      <c r="X13" s="9"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>41703</v>
       </c>
@@ -4701,59 +4805,68 @@
         <v>1.875</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>25.385000000000005</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="28">
+        <f t="shared" si="13"/>
+        <v>92.613748276541259</v>
+      </c>
+      <c r="K14" s="28">
+        <f t="shared" si="14"/>
+        <v>7.3862517234587335</v>
+      </c>
+      <c r="L14" s="9">
         <f>April2014LOI!R25</f>
         <v>6.8297355043100323</v>
       </c>
-      <c r="K14" s="9">
+      <c r="M14" s="9">
         <f>April2014LOI!S25</f>
         <v>78.493086765392135</v>
       </c>
-      <c r="L14" s="9">
+      <c r="N14" s="9">
         <f>April2014LOI!T25</f>
         <v>14.677177730297831</v>
       </c>
-      <c r="M14" s="9">
+      <c r="O14" s="9">
         <f>April2014LOI!U25</f>
         <v>9.8565263035110462</v>
       </c>
-      <c r="N14" s="9">
+      <c r="P14" s="9">
         <f>April2014LOI!V25</f>
         <v>65.640149305960421</v>
       </c>
-      <c r="O14" s="9">
+      <c r="Q14" s="9">
         <f>April2014LOI!W25</f>
         <v>24.503324390528533</v>
       </c>
-      <c r="P14" s="10">
-        <f t="shared" si="8"/>
+      <c r="R14" s="10">
+        <f t="shared" si="19"/>
         <v>3.4506044843930206</v>
       </c>
-      <c r="Q14" s="10">
-        <f t="shared" si="9"/>
+      <c r="S14" s="10">
+        <f t="shared" si="20"/>
         <v>0.45943733232241002</v>
       </c>
-      <c r="R14" s="10">
-        <f t="shared" si="10"/>
+      <c r="T14" s="10">
+        <f t="shared" si="21"/>
         <v>3.9100418167154305</v>
       </c>
-      <c r="S14" s="9">
-        <f t="shared" si="11"/>
-        <v>8.3431309039105397</v>
-      </c>
-      <c r="T14" s="9">
-        <f t="shared" si="12"/>
-        <v>72.066618035676271</v>
-      </c>
       <c r="U14" s="9">
-        <f t="shared" si="13"/>
-        <v>19.590251060413181</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>7.0533018918815067</v>
+      </c>
+      <c r="V14" s="9">
+        <f t="shared" si="16"/>
+        <v>77.543736450779789</v>
+      </c>
+      <c r="W14" s="9">
+        <f t="shared" si="17"/>
+        <v>15.402961657338704</v>
+      </c>
+      <c r="X14" s="9"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>41703</v>
       </c>
@@ -4781,59 +4894,68 @@
         <v>2.593</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>18.10700000000001</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="28">
+        <f t="shared" si="13"/>
+        <v>85.679571436461046</v>
+      </c>
+      <c r="K15" s="28">
+        <f t="shared" si="14"/>
+        <v>14.320428563538956</v>
+      </c>
+      <c r="L15" s="9">
         <f>April2014LOI!R27</f>
         <v>11.403250815377227</v>
       </c>
-      <c r="K15" s="9">
+      <c r="M15" s="9">
         <f>April2014LOI!S27</f>
         <v>33.926201678874996</v>
       </c>
-      <c r="L15" s="9">
+      <c r="N15" s="9">
         <f>April2014LOI!T27</f>
         <v>54.67054750574777</v>
       </c>
-      <c r="M15" s="9">
+      <c r="O15" s="9">
         <f>April2014LOI!U27</f>
         <v>9.4887348353552881</v>
       </c>
-      <c r="N15" s="9">
+      <c r="P15" s="9">
         <f>April2014LOI!V27</f>
         <v>28.129116117850852</v>
       </c>
-      <c r="O15" s="9">
+      <c r="Q15" s="9">
         <f>April2014LOI!W27</f>
         <v>62.382149046793856</v>
       </c>
-      <c r="P15" s="10">
-        <f t="shared" si="8"/>
+      <c r="R15" s="10">
+        <f t="shared" si="19"/>
         <v>8.4815887400417136</v>
       </c>
-      <c r="Q15" s="10">
-        <f t="shared" si="9"/>
+      <c r="S15" s="10">
+        <f t="shared" si="20"/>
         <v>1.6175691247833646</v>
       </c>
-      <c r="R15" s="10">
-        <f t="shared" si="10"/>
+      <c r="T15" s="10">
+        <f t="shared" si="21"/>
         <v>10.099157864825077</v>
       </c>
-      <c r="S15" s="9">
-        <f t="shared" si="11"/>
-        <v>10.445992825366258</v>
-      </c>
-      <c r="T15" s="9">
-        <f t="shared" si="12"/>
-        <v>31.027658898362922</v>
-      </c>
       <c r="U15" s="9">
-        <f t="shared" si="13"/>
-        <v>58.526348276270809</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>11.129083922120646</v>
+      </c>
+      <c r="V15" s="9">
+        <f t="shared" si="16"/>
+        <v>33.096034182341299</v>
+      </c>
+      <c r="W15" s="9">
+        <f t="shared" si="17"/>
+        <v>55.774881895538044</v>
+      </c>
+      <c r="X15" s="9"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>41703</v>
       </c>
@@ -4861,59 +4983,68 @@
         <v>1.6038999999999999</v>
       </c>
       <c r="I16" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>6.7278999999999947</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="28">
+        <f t="shared" si="13"/>
+        <v>76.16046611869973</v>
+      </c>
+      <c r="K16" s="28">
+        <f t="shared" si="14"/>
+        <v>23.839533881300273</v>
+      </c>
+      <c r="L16" s="9">
         <f>April2014LOI!R29</f>
         <v>6.3496816176617594</v>
       </c>
-      <c r="K16" s="9">
+      <c r="M16" s="9">
         <f>April2014LOI!S29</f>
         <v>87.638122043236152</v>
       </c>
-      <c r="L16" s="9">
+      <c r="N16" s="9">
         <f>April2014LOI!T29</f>
         <v>6.0121963391020889</v>
       </c>
-      <c r="M16" s="9">
+      <c r="O16" s="9">
         <f>April2014LOI!U29</f>
         <v>8.8688410825815875</v>
       </c>
-      <c r="N16" s="9">
+      <c r="P16" s="9">
         <f>April2014LOI!V29</f>
         <v>80.403053435114103</v>
       </c>
-      <c r="O16" s="9">
+      <c r="Q16" s="9">
         <f>April2014LOI!W29</f>
         <v>10.72810548230431</v>
       </c>
-      <c r="P16" s="10">
-        <f t="shared" si="8"/>
+      <c r="R16" s="10">
+        <f t="shared" si="19"/>
         <v>0.30806494041559074</v>
       </c>
-      <c r="Q16" s="10">
-        <f t="shared" si="9"/>
+      <c r="S16" s="10">
+        <f t="shared" si="20"/>
         <v>0.17206808383067881</v>
       </c>
-      <c r="R16" s="10">
-        <f t="shared" si="10"/>
+      <c r="T16" s="10">
+        <f t="shared" si="21"/>
         <v>0.48013302424626958</v>
       </c>
-      <c r="S16" s="9">
-        <f t="shared" si="11"/>
-        <v>7.6092613501216739</v>
-      </c>
-      <c r="T16" s="9">
-        <f t="shared" si="12"/>
-        <v>84.020587739175127</v>
-      </c>
       <c r="U16" s="9">
-        <f t="shared" si="13"/>
-        <v>8.3701509107031988</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>6.9502374918253045</v>
+      </c>
+      <c r="V16" s="9">
+        <f t="shared" si="16"/>
+        <v>85.913315411067586</v>
+      </c>
+      <c r="W16" s="9">
+        <f t="shared" si="17"/>
+        <v>7.1364470971071192</v>
+      </c>
+      <c r="X16" s="9"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>41703</v>
       </c>
@@ -4941,59 +5072,68 @@
         <v>1.19</v>
       </c>
       <c r="I17" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>21.27</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="28">
+        <f t="shared" si="13"/>
+        <v>94.40526563234603</v>
+      </c>
+      <c r="K17" s="28">
+        <f t="shared" si="14"/>
+        <v>5.594734367653972</v>
+      </c>
+      <c r="L17" s="9">
         <f>April2014LOI!R31</f>
         <v>7.4483508517579065</v>
       </c>
-      <c r="K17" s="9">
+      <c r="M17" s="9">
         <f>April2014LOI!S31</f>
         <v>77.63639776316468</v>
       </c>
-      <c r="L17" s="9">
+      <c r="N17" s="9">
         <f>April2014LOI!T31</f>
         <v>14.915251385077413</v>
       </c>
-      <c r="M17" s="9">
+      <c r="O17" s="9">
         <f>April2014LOI!U31</f>
         <v>9.5593497597381685</v>
       </c>
-      <c r="N17" s="9">
+      <c r="P17" s="9">
         <f>April2014LOI!V31</f>
         <v>73.15243840098185</v>
       </c>
-      <c r="O17" s="9">
+      <c r="Q17" s="9">
         <f>April2014LOI!W31</f>
         <v>17.288211839279981</v>
       </c>
-      <c r="P17" s="10">
-        <f t="shared" si="8"/>
+      <c r="R17" s="10">
+        <f t="shared" si="19"/>
         <v>2.9949824781235441</v>
       </c>
-      <c r="Q17" s="10">
-        <f t="shared" si="9"/>
+      <c r="S17" s="10">
+        <f t="shared" si="20"/>
         <v>0.20572972088743177</v>
       </c>
-      <c r="R17" s="10">
-        <f t="shared" si="10"/>
+      <c r="T17" s="10">
+        <f t="shared" si="21"/>
         <v>3.2007121990109759</v>
       </c>
-      <c r="S17" s="9">
-        <f t="shared" si="11"/>
-        <v>8.5038503057480384</v>
-      </c>
-      <c r="T17" s="9">
-        <f t="shared" si="12"/>
-        <v>75.394418082073258</v>
-      </c>
       <c r="U17" s="9">
-        <f t="shared" si="13"/>
-        <v>16.101731612178696</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>7.5664556331634785</v>
+      </c>
+      <c r="V17" s="9">
+        <f t="shared" si="16"/>
+        <v>77.385532147696992</v>
+      </c>
+      <c r="W17" s="9">
+        <f t="shared" si="17"/>
+        <v>15.048012219139522</v>
+      </c>
+      <c r="X17" s="9"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>41703</v>
       </c>
@@ -5021,59 +5161,68 @@
         <v>1.0110000000000001</v>
       </c>
       <c r="I18" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>40.311</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="28">
+        <f t="shared" si="13"/>
+        <v>97.491999702314502</v>
+      </c>
+      <c r="K18" s="28">
+        <f t="shared" si="14"/>
+        <v>2.5080002976854954</v>
+      </c>
+      <c r="L18" s="9">
         <f>April2014LOI!R33</f>
         <v>5.1305754564363131</v>
       </c>
-      <c r="K18" s="9">
+      <c r="M18" s="9">
         <f>April2014LOI!S33</f>
         <v>90.121937832216361</v>
       </c>
-      <c r="L18" s="9">
+      <c r="N18" s="9">
         <f>April2014LOI!T33</f>
         <v>4.7474867113473262</v>
       </c>
-      <c r="M18" s="9">
+      <c r="O18" s="9">
         <f>April2014LOI!U33</f>
         <v>7.9386110191013675</v>
       </c>
-      <c r="N18" s="9">
+      <c r="P18" s="9">
         <f>April2014LOI!V33</f>
         <v>83.962680799381346</v>
       </c>
-      <c r="O18" s="9">
+      <c r="Q18" s="9">
         <f>April2014LOI!W33</f>
         <v>8.0987081815172868</v>
       </c>
-      <c r="P18" s="10">
-        <f t="shared" si="8"/>
+      <c r="R18" s="10">
+        <f t="shared" si="19"/>
         <v>1.8657622775594991</v>
       </c>
-      <c r="Q18" s="10">
-        <f t="shared" si="9"/>
+      <c r="S18" s="10">
+        <f t="shared" si="20"/>
         <v>8.1877939715139778E-2</v>
       </c>
-      <c r="R18" s="10">
-        <f t="shared" si="10"/>
+      <c r="T18" s="10">
+        <f t="shared" si="21"/>
         <v>1.9476402172746388</v>
       </c>
-      <c r="S18" s="9">
-        <f t="shared" si="11"/>
-        <v>6.5345932377688403</v>
-      </c>
-      <c r="T18" s="9">
-        <f t="shared" si="12"/>
-        <v>87.04230931579886</v>
-      </c>
       <c r="U18" s="9">
-        <f t="shared" si="13"/>
-        <v>6.4230974464323065</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>5.2010009967070676</v>
+      </c>
+      <c r="V18" s="9">
+        <f t="shared" si="16"/>
+        <v>89.967463647497638</v>
+      </c>
+      <c r="W18" s="9">
+        <f t="shared" si="17"/>
+        <v>4.8315353557952889</v>
+      </c>
+      <c r="X18" s="9"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>41703</v>
       </c>
@@ -5101,59 +5250,68 @@
         <v>1.1780000000000002</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>30.728000000000012</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="28">
+        <f t="shared" si="13"/>
+        <v>96.16636292632127</v>
+      </c>
+      <c r="K19" s="28">
+        <f t="shared" si="14"/>
+        <v>3.8336370736787284</v>
+      </c>
+      <c r="L19" s="9">
         <f>April2014LOI!R35</f>
         <v>4.6182881947721039</v>
       </c>
-      <c r="K19" s="9">
+      <c r="M19" s="9">
         <f>April2014LOI!S35</f>
         <v>91.164159667830532</v>
       </c>
-      <c r="L19" s="9">
+      <c r="N19" s="9">
         <f>April2014LOI!T35</f>
         <v>4.2175521373973641</v>
       </c>
-      <c r="M19" s="9">
+      <c r="O19" s="9">
         <f>April2014LOI!U35</f>
         <v>7.9017460787214988</v>
       </c>
-      <c r="N19" s="9">
+      <c r="P19" s="9">
         <f>April2014LOI!V35</f>
         <v>83.638650488310532</v>
       </c>
-      <c r="O19" s="9">
+      <c r="Q19" s="9">
         <f>April2014LOI!W35</f>
         <v>8.4596034329679703</v>
       </c>
-      <c r="P19" s="10">
-        <f t="shared" si="8"/>
+      <c r="R19" s="10">
+        <f t="shared" si="19"/>
         <v>1.2462866566009216</v>
       </c>
-      <c r="Q19" s="10">
-        <f t="shared" si="9"/>
+      <c r="S19" s="10">
+        <f t="shared" si="20"/>
         <v>9.9654128440362699E-2</v>
       </c>
-      <c r="R19" s="10">
-        <f t="shared" si="10"/>
+      <c r="T19" s="10">
+        <f t="shared" si="21"/>
         <v>1.3459407850412843</v>
       </c>
-      <c r="S19" s="9">
-        <f t="shared" si="11"/>
-        <v>6.2600171367468018</v>
-      </c>
-      <c r="T19" s="9">
-        <f>(K19+N19)/2</f>
-        <v>87.401405078070525</v>
-      </c>
       <c r="U19" s="9">
-        <f t="shared" si="13"/>
-        <v>6.3385777851826672</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>4.7441640535098148</v>
+      </c>
+      <c r="V19" s="9">
+        <f t="shared" si="16"/>
+        <v>90.875658957941354</v>
+      </c>
+      <c r="W19" s="9">
+        <f t="shared" si="17"/>
+        <v>4.3801769885488273</v>
+      </c>
+      <c r="X19" s="9"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>41703</v>
       </c>
@@ -5181,64 +5339,73 @@
         <v>1.2210000000000001</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>2.4529999999999994</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="28">
+        <f t="shared" si="13"/>
+        <v>50.22421524663676</v>
+      </c>
+      <c r="K20" s="28">
+        <f t="shared" si="14"/>
+        <v>49.775784753363247</v>
+      </c>
+      <c r="L20" s="9">
         <f>April2014LOI!R37</f>
         <v>10.351893095768457</v>
       </c>
-      <c r="K20" s="9">
+      <c r="M20" s="9">
         <f>April2014LOI!S37</f>
         <v>80.58752783964367</v>
       </c>
-      <c r="L20" s="9">
+      <c r="N20" s="9">
         <f>April2014LOI!T37</f>
         <v>9.0605790645878734</v>
       </c>
-      <c r="M20" s="9">
+      <c r="O20" s="9">
         <f>April2014LOI!U37</f>
         <v>8.079748163693413</v>
       </c>
-      <c r="N20" s="9">
+      <c r="P20" s="9">
         <f>April2014LOI!V37</f>
         <v>79.362300868072609</v>
       </c>
-      <c r="O20" s="9">
+      <c r="Q20" s="9">
         <f>April2014LOI!W37</f>
         <v>12.557950968233978</v>
       </c>
-      <c r="P20" s="10">
-        <f t="shared" si="8"/>
+      <c r="R20" s="10">
+        <f t="shared" si="19"/>
         <v>0.11162633407572253</v>
       </c>
-      <c r="Q20" s="10">
-        <f t="shared" si="9"/>
+      <c r="S20" s="10">
+        <f t="shared" si="20"/>
         <v>0.15333258132213687</v>
       </c>
-      <c r="R20" s="10">
-        <f t="shared" si="10"/>
+      <c r="T20" s="10">
+        <f t="shared" si="21"/>
         <v>0.26495891539785943</v>
       </c>
-      <c r="S20" s="9">
-        <f t="shared" si="11"/>
-        <v>9.2158206297309349</v>
-      </c>
-      <c r="T20" s="9">
-        <f t="shared" si="12"/>
-        <v>79.974914353858139</v>
-      </c>
       <c r="U20" s="9">
-        <f t="shared" si="13"/>
-        <v>10.809265016410926</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>9.2209151250943311</v>
+      </c>
+      <c r="V20" s="9">
+        <f t="shared" si="16"/>
+        <v>79.977661499534321</v>
+      </c>
+      <c r="W20" s="9">
+        <f t="shared" si="17"/>
+        <v>10.801423375371362</v>
+      </c>
+      <c r="X20" s="9"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added S2C coarse fraction for April
Jamo sent the missing data
</commit_message>
<xml_diff>
--- a/Data/CRCP Sediment Data.xlsx
+++ b/Data/CRCP Sediment Data.xlsx
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">April2014LOI!$A$2:$T$38</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
   <si>
     <t>Location</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>T1C</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>NAN</t>
@@ -809,7 +806,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.306930693068642</c:v>
+                  <c:v>7.6583728607523511</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="@">
                   <c:v>0</c:v>
@@ -931,7 +928,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>86.97920792079222</c:v>
+                  <c:v>80.197948146324947</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="@">
                   <c:v>0</c:v>
@@ -1050,7 +1047,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7138613861391381</c:v>
+                  <c:v>12.143678992922702</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="@">
                   <c:v>0</c:v>
@@ -1075,8 +1072,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="284250856"/>
-        <c:axId val="284252816"/>
+        <c:axId val="330858040"/>
+        <c:axId val="330860000"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1207,7 +1204,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16799999999999993</c:v>
+                  <c:v>3.5660000000000034</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1233,11 +1230,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="284253208"/>
-        <c:axId val="284249288"/>
+        <c:axId val="330862744"/>
+        <c:axId val="330859216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="284250856"/>
+        <c:axId val="330858040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1280,7 +1277,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284252816"/>
+        <c:crossAx val="330860000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1288,7 +1285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="284252816"/>
+        <c:axId val="330860000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,12 +1336,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284250856"/>
+        <c:crossAx val="330858040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="284249288"/>
+        <c:axId val="330859216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,12 +1378,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284253208"/>
+        <c:crossAx val="330862744"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="284253208"/>
+        <c:axId val="330862744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1396,7 +1393,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="284249288"/>
+        <c:crossAx val="330859216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1955,8 +1952,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="284254384"/>
-        <c:axId val="284255560"/>
+        <c:axId val="330860392"/>
+        <c:axId val="330864704"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2039,11 +2036,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="285608016"/>
-        <c:axId val="284248504"/>
+        <c:axId val="330861176"/>
+        <c:axId val="330858432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="284254384"/>
+        <c:axId val="330860392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2086,7 +2083,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284255560"/>
+        <c:crossAx val="330864704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2094,7 +2091,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="284255560"/>
+        <c:axId val="330864704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2145,12 +2142,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284254384"/>
+        <c:crossAx val="330860392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="284248504"/>
+        <c:axId val="330858432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2187,12 +2184,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="285608016"/>
+        <c:crossAx val="330861176"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="285608016"/>
+        <c:axId val="330861176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2201,7 +2198,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="284248504"/>
+        <c:crossAx val="330858432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3717,11 +3714,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E1" sqref="E1"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
-      <selection pane="bottomRight" activeCell="AG21" sqref="AG21"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3749,16 +3742,16 @@
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>120</v>
-      </c>
       <c r="C2" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>117</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>118</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>0</v>
@@ -3767,55 +3760,55 @@
         <v>1</v>
       </c>
       <c r="G2" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="L2" s="24" t="s">
+      <c r="O2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="P2" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q2" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" s="24" t="s">
+      <c r="S2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="T2" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="T2" s="24" t="s">
-        <v>51</v>
-      </c>
       <c r="U2" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="V2" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="V2" s="19" t="s">
+      <c r="W2" s="19" t="s">
         <v>115</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -4248,15 +4241,15 @@
         <v>0</v>
       </c>
       <c r="U7" s="9">
-        <f t="shared" ref="U4:U8" si="9">(L7*J7/100+O7*K7/100)</f>
+        <f t="shared" ref="U7" si="9">(L7*J7/100+O7*K7/100)</f>
         <v>0</v>
       </c>
       <c r="V7" s="9">
-        <f t="shared" ref="V4:V11" si="10">(M7+P7)/2</f>
+        <f t="shared" ref="V7:V11" si="10">(M7+P7)/2</f>
         <v>0</v>
       </c>
       <c r="W7" s="9">
-        <f t="shared" ref="W4:W11" si="11">(N7+Q7)/2</f>
+        <f t="shared" ref="W7:W11" si="11">(N7+Q7)/2</f>
         <v>0</v>
       </c>
       <c r="X7" s="9"/>
@@ -4281,7 +4274,8 @@
         <v>11</v>
       </c>
       <c r="G8" s="10">
-        <v>0</v>
+        <f>April2014!D11</f>
+        <v>3.3980000000000032</v>
       </c>
       <c r="H8" s="10">
         <f>April2014!H11</f>
@@ -4289,15 +4283,15 @@
       </c>
       <c r="I8" s="10">
         <f t="shared" si="0"/>
-        <v>0.16799999999999993</v>
+        <v>3.5660000000000034</v>
       </c>
       <c r="J8" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>(G8/I8)*100</f>
+        <v>95.288839035333709</v>
       </c>
       <c r="K8" s="28">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f>(H8/I8)*100</f>
+        <v>4.711160964666286</v>
       </c>
       <c r="L8" s="9">
         <f>April2014LOI!R12</f>
@@ -4325,7 +4319,7 @@
       </c>
       <c r="R8" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.42680430575891021</v>
       </c>
       <c r="S8" s="10">
         <f t="shared" si="4"/>
@@ -4333,19 +4327,19 @@
       </c>
       <c r="T8" s="10">
         <f t="shared" si="5"/>
-        <v>6.2392871287137493E-3</v>
+        <v>0.43304359288762395</v>
       </c>
       <c r="U8" s="9">
         <f>(L8*$J8/100+O8*$K8/100)</f>
-        <v>9.306930693068642</v>
+        <v>7.6583728607523511</v>
       </c>
       <c r="V8" s="9">
         <f>(M8*$J8/100+P8*$K8/100)</f>
-        <v>86.97920792079222</v>
+        <v>80.197948146324947</v>
       </c>
       <c r="W8" s="9">
         <f>(N8*$J8/100+Q8*$K8/100)</f>
-        <v>3.7138613861391381</v>
+        <v>12.143678992922702</v>
       </c>
       <c r="X8" s="9"/>
     </row>
@@ -4377,13 +4371,13 @@
         <v>NAN</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L9" s="10" t="str">
         <f>April2014!G12</f>
@@ -4394,34 +4388,34 @@
         <v>NAN</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X9" s="9"/>
     </row>
@@ -4499,7 +4493,7 @@
         <v>0</v>
       </c>
       <c r="U10" s="9">
-        <f t="shared" ref="U4:U11" si="12">(L10+O10)/2</f>
+        <f t="shared" ref="U10:U11" si="12">(L10+O10)/2</f>
         <v>0</v>
       </c>
       <c r="V10" s="9">
@@ -4631,11 +4625,11 @@
         <v>10.683999999999997</v>
       </c>
       <c r="J12" s="28">
-        <f t="shared" ref="J10:J20" si="13">(G12/I12)*100</f>
+        <f t="shared" ref="J12:J20" si="13">(G12/I12)*100</f>
         <v>84.902658180456754</v>
       </c>
       <c r="K12" s="28">
-        <f t="shared" ref="K10:K20" si="14">(H12/I12)*100</f>
+        <f t="shared" ref="K12:K20" si="14">(H12/I12)*100</f>
         <v>15.097341819543248</v>
       </c>
       <c r="L12" s="9">
@@ -5437,81 +5431,81 @@
   <sheetData>
     <row r="1" spans="1:23" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="S1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="R1" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="T1" s="15" t="s">
-        <v>72</v>
-      </c>
       <c r="U1" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V1" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="15" t="s">
         <v>71</v>
-      </c>
-      <c r="W1" s="15" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="16">
         <v>41741</v>
@@ -5594,10 +5588,10 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="16">
         <v>41741</v>
@@ -5668,10 +5662,10 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" s="16">
         <v>41741</v>
@@ -5754,10 +5748,10 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="16">
         <v>41741</v>
@@ -5828,10 +5822,10 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="16">
         <v>41741</v>
@@ -5914,10 +5908,10 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="16">
         <v>41741</v>
@@ -5988,10 +5982,10 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="16">
         <v>41741</v>
@@ -6074,10 +6068,10 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="16">
         <v>41741</v>
@@ -6148,10 +6142,10 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -6175,10 +6169,10 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -6190,10 +6184,10 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="16">
         <v>41741</v>
@@ -6276,10 +6270,10 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="16">
         <v>41741</v>
@@ -6350,10 +6344,10 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
@@ -6377,10 +6371,10 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -6392,10 +6386,10 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -6419,10 +6413,10 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -6434,10 +6428,10 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -6461,10 +6455,10 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -6485,10 +6479,10 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="16">
         <v>41741</v>
@@ -6571,10 +6565,10 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="16">
         <v>41741</v>
@@ -6645,10 +6639,10 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="16">
         <v>41741</v>
@@ -6731,10 +6725,10 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" s="16">
         <v>41741</v>
@@ -6805,10 +6799,10 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="16">
         <v>41741</v>
@@ -6891,10 +6885,10 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C26" s="16">
         <v>41741</v>
@@ -6965,10 +6959,10 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" s="16">
         <v>41741</v>
@@ -7051,10 +7045,10 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" s="16">
         <v>41741</v>
@@ -7125,10 +7119,10 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C29" s="16">
         <v>41741</v>
@@ -7211,10 +7205,10 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" s="16">
         <v>41741</v>
@@ -7285,10 +7279,10 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" s="16">
         <v>41741</v>
@@ -7371,10 +7365,10 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="16">
         <v>41741</v>
@@ -7445,10 +7439,10 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C33" s="16">
         <v>41741</v>
@@ -7531,10 +7525,10 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C34" s="16">
         <v>41741</v>
@@ -7605,10 +7599,10 @@
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C35" s="16">
         <v>41741</v>
@@ -7691,10 +7685,10 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" s="16">
         <v>41741</v>
@@ -7765,10 +7759,10 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C37" s="16">
         <v>41741</v>
@@ -7851,10 +7845,10 @@
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" s="16">
         <v>41741</v>
@@ -7949,8 +7943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8124,13 +8118,14 @@
         <v>22</v>
       </c>
       <c r="B11" s="6">
-        <v>66.997</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>40</v>
+        <v>49.908999999999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>53.307000000000002</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" ref="D11" si="0">C11-B11</f>
+        <v>3.3980000000000032</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="8">
@@ -8146,26 +8141,26 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -8239,7 +8234,7 @@
         <v>78.757999999999996</v>
       </c>
       <c r="D16" s="7">
-        <f t="shared" ref="D16:D24" si="0">C16-B16</f>
+        <f t="shared" ref="D16:D24" si="1">C16-B16</f>
         <v>9.070999999999998</v>
       </c>
       <c r="E16" s="4"/>
@@ -8250,7 +8245,7 @@
         <v>3.3410000000000002</v>
       </c>
       <c r="H16" s="6">
-        <f t="shared" ref="H16:H24" si="1">G16-F16</f>
+        <f t="shared" ref="H16:H24" si="2">G16-F16</f>
         <v>1.6130000000000002</v>
       </c>
     </row>
@@ -8265,7 +8260,7 @@
         <v>110.946</v>
       </c>
       <c r="D17" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44.081999999999994</v>
       </c>
       <c r="E17" s="4"/>
@@ -8276,7 +8271,7 @@
         <v>4.3150000000000004</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6300000000000003</v>
       </c>
     </row>
@@ -8291,7 +8286,7 @@
         <v>106.504</v>
       </c>
       <c r="D18" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23.510000000000005</v>
       </c>
       <c r="E18" s="4"/>
@@ -8302,7 +8297,7 @@
         <v>3.597</v>
       </c>
       <c r="H18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.875</v>
       </c>
     </row>
@@ -8317,7 +8312,7 @@
         <v>85.715000000000003</v>
       </c>
       <c r="D19" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.51400000000001</v>
       </c>
       <c r="E19" s="4"/>
@@ -8328,7 +8323,7 @@
         <v>4.3739999999999997</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.593</v>
       </c>
     </row>
@@ -8343,7 +8338,7 @@
         <v>73.19</v>
       </c>
       <c r="D20" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1239999999999952</v>
       </c>
       <c r="E20" s="4"/>
@@ -8354,7 +8349,7 @@
         <v>3.3369</v>
       </c>
       <c r="H20" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6038999999999999</v>
       </c>
     </row>
@@ -8369,7 +8364,7 @@
         <v>89.942999999999998</v>
       </c>
       <c r="D21" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.079999999999998</v>
       </c>
       <c r="E21" s="4"/>
@@ -8380,7 +8375,7 @@
         <v>2.9239999999999999</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.19</v>
       </c>
     </row>
@@ -8395,7 +8390,7 @@
         <v>106.73099999999999</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39.299999999999997</v>
       </c>
       <c r="E22" s="4"/>
@@ -8406,7 +8401,7 @@
         <v>2.7690000000000001</v>
       </c>
       <c r="H22" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0110000000000001</v>
       </c>
     </row>
@@ -8421,7 +8416,7 @@
         <v>99.766000000000005</v>
       </c>
       <c r="D23" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29.550000000000011</v>
       </c>
       <c r="E23" s="4"/>
@@ -8432,7 +8427,7 @@
         <v>2.8730000000000002</v>
       </c>
       <c r="H23" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1780000000000002</v>
       </c>
     </row>
@@ -8447,7 +8442,7 @@
         <v>67.570999999999998</v>
       </c>
       <c r="D24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2319999999999993</v>
       </c>
       <c r="E24" s="4"/>
@@ -8458,7 +8453,7 @@
         <v>2.9670000000000001</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2210000000000001</v>
       </c>
     </row>

</xml_diff>